<commit_message>
Random with different groups
</commit_message>
<xml_diff>
--- a/src/main/java/stas/documents/fileExcel.xlsx
+++ b/src/main/java/stas/documents/fileExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stasf\IdeaProjects\Randomizer\src\main\java\stas\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IdeaProjects\Randomizer\src\main\java\stas\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82393CFD-6545-4D88-894A-13417586CF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4C7936-A26D-4DCD-91AB-9630FD174126}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5977ACB3-F08E-4C56-9D2A-BDA913716221}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{5977ACB3-F08E-4C56-9D2A-BDA913716221}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,6 @@
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -417,15 +416,15 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -436,7 +435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1+1</f>
         <v>2</v>
@@ -448,7 +447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A10" si="0">A2+1</f>
         <v>3</v>
@@ -460,7 +459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -472,7 +471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -484,7 +483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -496,7 +495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -508,7 +507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -517,10 +516,10 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -532,7 +531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>10</v>

</xml_diff>